<commit_message>
CP317 - Final Commit (pre check)
</commit_message>
<xml_diff>
--- a/CP317/Project/text_execution.xlsx
+++ b/CP317/Project/text_execution.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RjKim\dev\Year3Sem2\CP317\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FA1B17-7CC1-47B1-8789-F170AAE11484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF1EB28-B709-4E42-99E7-54AC8B0F582D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57710" yWindow="-4600" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Test Number</t>
   </si>
@@ -88,13 +88,16 @@
   </si>
   <si>
     <t>The program has the functionality to properly checkout  a new book.</t>
+  </si>
+  <si>
+    <t>Ryan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,8 +120,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -128,6 +138,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -179,12 +194,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1"/>
@@ -198,9 +214,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,6 +545,13 @@
       <c r="C2" s="8" t="s">
         <v>15</v>
       </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="3">
+        <v>45024</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -538,6 +563,13 @@
       <c r="C3" s="8" t="s">
         <v>16</v>
       </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="3">
+        <v>45024</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -549,6 +581,13 @@
       <c r="C4" s="8" t="s">
         <v>17</v>
       </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="3">
+        <v>45024</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -560,6 +599,13 @@
       <c r="C5" s="8" t="s">
         <v>18</v>
       </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="3">
+        <v>45024</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -571,6 +617,13 @@
       <c r="C6" s="8" t="s">
         <v>19</v>
       </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="3">
+        <v>45024</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -582,14 +635,30 @@
       <c r="C7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="9"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="3">
+        <v>45024</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>14</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="3">
+        <v>45024</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>